<commit_message>
rechecked the referred mic and disk RIS
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_data_summary_referred_2023.xlsx
+++ b/whonet/static/whonet_xl/whonet_data_summary_referred_2023.xlsx
@@ -19,9 +19,12 @@
     <sheet name="efa_efm" sheetId="5" r:id="rId5"/>
     <sheet name="sau" sheetId="6" r:id="rId6"/>
     <sheet name="sal_shi" sheetId="7" r:id="rId7"/>
-    <sheet name="ngo" sheetId="8" r:id="rId8"/>
+    <sheet name="hin_hpn" sheetId="9" r:id="rId8"/>
+    <sheet name="ngo" sheetId="8" r:id="rId9"/>
+    <sheet name="nme" sheetId="12" r:id="rId10"/>
+    <sheet name="bs-" sheetId="14" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="102">
   <si>
     <t>ORGNAME</t>
   </si>
@@ -138,9 +141,6 @@
     <t>Cefotaxime</t>
   </si>
   <si>
-    <t>CTZ_NM</t>
-  </si>
-  <si>
     <t>CRO_ND30</t>
   </si>
   <si>
@@ -253,12 +253,102 @@
   </si>
   <si>
     <t>ngo</t>
+  </si>
+  <si>
+    <t>hin,hpn</t>
+  </si>
+  <si>
+    <t>Ampicillin</t>
+  </si>
+  <si>
+    <t>Amoxicillin-clavulanic acid</t>
+  </si>
+  <si>
+    <t>Levofloxacin</t>
+  </si>
+  <si>
+    <t>Cefixime</t>
+  </si>
+  <si>
+    <t>nme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rifampin </t>
+  </si>
+  <si>
+    <t>Penicillin</t>
+  </si>
+  <si>
+    <t>Daptomycin</t>
+  </si>
+  <si>
+    <t>bs-</t>
+  </si>
+  <si>
+    <t>AMP_ND10</t>
+  </si>
+  <si>
+    <t>AMC_NM</t>
+  </si>
+  <si>
+    <t>LVX_ND5</t>
+  </si>
+  <si>
+    <t>AMP_NM</t>
+  </si>
+  <si>
+    <t>LVX_NM</t>
+  </si>
+  <si>
+    <t>CFM_ND5</t>
+  </si>
+  <si>
+    <t>CFM_NM</t>
+  </si>
+  <si>
+    <t>RIF_ND5</t>
+  </si>
+  <si>
+    <t>RIF_NM</t>
+  </si>
+  <si>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>PEN_ND10</t>
+  </si>
+  <si>
+    <t>DAP_ND-</t>
+  </si>
+  <si>
+    <t>PEN_NM</t>
+  </si>
+  <si>
+    <t>DAP_NM</t>
+  </si>
+  <si>
+    <t>AMC_ND20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -280,7 +370,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +392,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -359,6 +455,38 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -644,7 +772,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,10 +828,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5">
@@ -718,7 +846,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2" s="6">
         <v>64</v>
@@ -952,7 +1080,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="K9" s="4">
         <v>4</v>
@@ -966,10 +1094,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>22</v>
@@ -986,7 +1114,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10" s="4">
         <v>4</v>
@@ -1000,10 +1128,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4">
@@ -1018,7 +1146,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" s="4">
         <v>16</v>
@@ -1030,6 +1158,447 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="10">
+        <v>5</v>
+      </c>
+      <c r="F2" s="9">
+        <v>32</v>
+      </c>
+      <c r="G2" s="9">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="L2" s="9">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="10">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="10">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9">
+        <v>19</v>
+      </c>
+      <c r="G4" s="9">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" s="9">
+        <v>2</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="10">
+        <v>30</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9">
+        <v>0.125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.42578125" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="10">
+        <v>10</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="10">
+        <v>10</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="10">
+        <v>30</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="10">
+        <v>30</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="10">
+        <v>30</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="J7" t="s">
+        <v>100</v>
+      </c>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="10">
+        <v>30</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="10">
+        <v>30</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1038,345 +1607,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="4">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4">
-        <v>15</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="4">
-        <v>16</v>
-      </c>
-      <c r="L2" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4">
-        <v>12</v>
-      </c>
-      <c r="G3" s="4">
-        <v>15</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="4">
-        <v>16</v>
-      </c>
-      <c r="L3" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="4">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4">
-        <v>19</v>
-      </c>
-      <c r="G4" s="4">
-        <v>23</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="4">
-        <v>4</v>
-      </c>
-      <c r="L4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4">
-        <v>10</v>
-      </c>
-      <c r="F5" s="4">
-        <v>19</v>
-      </c>
-      <c r="G5" s="4">
-        <v>23</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="4">
-        <v>4</v>
-      </c>
-      <c r="L5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4">
-        <v>10</v>
-      </c>
-      <c r="F6" s="4">
-        <v>18</v>
-      </c>
-      <c r="G6" s="4">
-        <v>22</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="4">
-        <v>2</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="4">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4">
-        <v>18</v>
-      </c>
-      <c r="G2" s="4">
-        <v>22</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="4">
-        <v>8</v>
-      </c>
-      <c r="L2" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4">
-        <v>14</v>
-      </c>
-      <c r="G3" s="4">
-        <v>18</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="4">
-        <v>8</v>
-      </c>
-      <c r="L3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,15 +1654,381 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="4">
+        <v>16</v>
+      </c>
+      <c r="L2" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="4">
+        <v>16</v>
+      </c>
+      <c r="L3" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4">
+        <v>23</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="4">
+        <v>4</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4">
+        <v>19</v>
+      </c>
+      <c r="G5" s="4">
+        <v>23</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="4">
+        <v>4</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4">
+        <v>22</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9:H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4">
+        <v>22</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="4">
+        <v>8</v>
+      </c>
+      <c r="L2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="4">
+        <v>8</v>
+      </c>
+      <c r="L3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5">
@@ -1446,7 +2043,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K2" s="6">
         <v>64</v>
@@ -1457,7 +2054,7 @@
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>13</v>
@@ -1489,9 +2086,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>19</v>
@@ -1525,7 +2122,7 @@
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>21</v>
@@ -1559,7 +2156,7 @@
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>25</v>
@@ -1599,7 +2196,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1651,13 +2248,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5">
@@ -1672,7 +2269,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K2" s="6">
         <v>513</v>
@@ -1683,13 +2280,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>15</v>
@@ -1706,7 +2303,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K3" s="4">
         <v>1025</v>
@@ -1717,13 +2314,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
@@ -1740,7 +2337,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K4" s="4">
         <v>8</v>
@@ -1751,13 +2348,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>22</v>
@@ -1774,7 +2371,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K5" s="4">
         <v>32</v>
@@ -1848,13 +2445,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5">
@@ -1869,7 +2466,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K2" s="6">
         <v>4</v>
@@ -1880,13 +2477,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4">
@@ -1901,7 +2498,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K3" s="4">
         <v>8</v>
@@ -1920,13 +2517,23 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L5"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1969,13 +2576,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5">
@@ -1990,7 +2597,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K2" s="6">
         <v>1</v>
@@ -2001,13 +2608,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4">
@@ -2022,7 +2629,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K3" s="4">
         <v>32</v>
@@ -2033,7 +2640,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>34</v>
@@ -2054,7 +2661,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K4" s="4">
         <v>4</v>
@@ -2065,13 +2672,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4">
@@ -2086,7 +2693,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" s="4">
         <v>4</v>
@@ -2102,10 +2709,233 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="10">
+        <v>10</v>
+      </c>
+      <c r="F2" s="12">
+        <v>18</v>
+      </c>
+      <c r="G2" s="12">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="12">
+        <v>4</v>
+      </c>
+      <c r="L2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="J3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="12">
+        <v>8</v>
+      </c>
+      <c r="L3" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="10">
+        <v>5</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="10">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="10">
+        <v>30</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="10">
+        <v>10</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,6 +2943,15 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2155,67 +2994,119 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="E2" s="5">
+        <v>15</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11">
+        <v>30</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="J2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="E3" s="4">
+        <v>5</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9">
+        <v>31</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+      <c r="J3" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="16">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="E4" s="4">
+        <v>30</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9">
+        <v>35</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
+      <c r="J4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="9"/>
+      <c r="L4" s="16">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="E5" s="4">
+        <v>5</v>
+      </c>
+      <c r="F5" s="9">
+        <v>27</v>
+      </c>
+      <c r="G5" s="9">
+        <v>41</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="J5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="9">
+        <v>1</v>
+      </c>
+      <c r="L5" s="15">
+        <v>6.4000000000000001E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check for the bug DAP_ND-
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_data_summary_referred_2023.xlsx
+++ b/whonet/static/whonet_xl/whonet_data_summary_referred_2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="eco" sheetId="1" r:id="rId1"/>
@@ -330,9 +330,6 @@
     <t>PEN_ND10</t>
   </si>
   <si>
-    <t>DAP_ND-</t>
-  </si>
-  <si>
     <t>PEN_NM</t>
   </si>
   <si>
@@ -340,6 +337,9 @@
   </si>
   <si>
     <t>AMC_ND20</t>
+  </si>
+  <si>
+    <t>DAP_ND30</t>
   </si>
 </sst>
 </file>
@@ -771,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1340,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,7 +1440,7 @@
         <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K3" s="20"/>
       <c r="L3" s="20" t="s">
@@ -1530,7 +1530,7 @@
         <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>95</v>
@@ -1540,7 +1540,7 @@
         <v>95</v>
       </c>
       <c r="J7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
@@ -2806,7 +2806,7 @@
         <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="13"/>

</xml_diff>

<commit_message>
updated whonet data summary
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_data_summary_referred_2023.xlsx
+++ b/whonet/static/whonet_xl/whonet_data_summary_referred_2023.xlsx
@@ -9,20 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="eco" sheetId="1" r:id="rId1"/>
     <sheet name="kpn" sheetId="2" r:id="rId2"/>
     <sheet name="aba" sheetId="3" r:id="rId3"/>
     <sheet name="pae" sheetId="4" r:id="rId4"/>
-    <sheet name="efa_efm" sheetId="5" r:id="rId5"/>
-    <sheet name="sau" sheetId="6" r:id="rId6"/>
-    <sheet name="sal_shi" sheetId="7" r:id="rId7"/>
-    <sheet name="hin_hpn" sheetId="9" r:id="rId8"/>
-    <sheet name="ngo" sheetId="8" r:id="rId9"/>
-    <sheet name="nme" sheetId="12" r:id="rId10"/>
-    <sheet name="bs-" sheetId="14" r:id="rId11"/>
+    <sheet name="pma" sheetId="15" r:id="rId5"/>
+    <sheet name="efa_efm" sheetId="5" r:id="rId6"/>
+    <sheet name="sau" sheetId="6" r:id="rId7"/>
+    <sheet name="sal_shi" sheetId="7" r:id="rId8"/>
+    <sheet name="hin_hpn" sheetId="9" r:id="rId9"/>
+    <sheet name="ngo" sheetId="8" r:id="rId10"/>
+    <sheet name="nme" sheetId="12" r:id="rId11"/>
+    <sheet name="spn" sheetId="16" r:id="rId12"/>
+    <sheet name="bs-" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="137">
   <si>
     <t>ORGNAME</t>
   </si>
@@ -321,9 +323,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -340,6 +339,114 @@
   </si>
   <si>
     <t>DAP_ND30</t>
+  </si>
+  <si>
+    <t>Ceftazidime-avibactam</t>
+  </si>
+  <si>
+    <t>CZA_ND30</t>
+  </si>
+  <si>
+    <t>CZA_NM</t>
+  </si>
+  <si>
+    <t>Imipenem-relebactam</t>
+  </si>
+  <si>
+    <t>IMR_ND10</t>
+  </si>
+  <si>
+    <t>IMR_NM</t>
+  </si>
+  <si>
+    <t>Meropenem-vaborbactam</t>
+  </si>
+  <si>
+    <t>MEV_ND20</t>
+  </si>
+  <si>
+    <t>MEV_NM</t>
+  </si>
+  <si>
+    <t>Cefiderocol</t>
+  </si>
+  <si>
+    <t>FDC_ND</t>
+  </si>
+  <si>
+    <t>FDC_NM</t>
+  </si>
+  <si>
+    <t>Plazomicin</t>
+  </si>
+  <si>
+    <t>PLZ_ND</t>
+  </si>
+  <si>
+    <t>PLZ_NM</t>
+  </si>
+  <si>
+    <t>CZT_ND30</t>
+  </si>
+  <si>
+    <t>CZT_NM</t>
+  </si>
+  <si>
+    <t>Ceftolozane-tazobactam</t>
+  </si>
+  <si>
+    <t>Trimethoprim-sulfaethoxazole</t>
+  </si>
+  <si>
+    <t>SXT_ND1_2</t>
+  </si>
+  <si>
+    <t>SXT_NM</t>
+  </si>
+  <si>
+    <t>pma</t>
+  </si>
+  <si>
+    <t>Tedizolid</t>
+  </si>
+  <si>
+    <t>TZD_ND</t>
+  </si>
+  <si>
+    <t>TZD_NM</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>Ampicilin</t>
+  </si>
+  <si>
+    <t>Oxacillin</t>
+  </si>
+  <si>
+    <t>OXA_ND1</t>
+  </si>
+  <si>
+    <t>OXA_NM</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>Penicilin</t>
+  </si>
+  <si>
+    <t>spn</t>
+  </si>
+  <si>
+    <t>Amoxicillin</t>
+  </si>
+  <si>
+    <t>AMX_ND30</t>
+  </si>
+  <si>
+    <t>AMX_NM</t>
   </si>
 </sst>
 </file>
@@ -402,7 +509,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -425,12 +532,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -468,7 +586,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -486,6 +603,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -769,16 +917,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -838,10 +986,10 @@
         <v>30</v>
       </c>
       <c r="F2" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G2" s="5">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -849,10 +997,10 @@
         <v>46</v>
       </c>
       <c r="K2" s="6">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="L2" s="6">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -872,10 +1020,10 @@
         <v>10</v>
       </c>
       <c r="F3" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -883,10 +1031,10 @@
         <v>16</v>
       </c>
       <c r="K3" s="4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L3" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -909,7 +1057,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -917,10 +1065,10 @@
         <v>17</v>
       </c>
       <c r="K4" s="4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L4" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1152,6 +1300,148 @@
         <v>16</v>
       </c>
       <c r="L11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="1">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1">
+        <v>21</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L12" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="1">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1">
+        <v>25</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K13" s="1">
+        <v>4</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="1">
+        <v>20</v>
+      </c>
+      <c r="F14" s="1">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1">
+        <v>18</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K14" s="1">
+        <v>16</v>
+      </c>
+      <c r="L14" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="1">
+        <v>30</v>
+      </c>
+      <c r="F15" s="1">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1">
+        <v>16</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K15" s="1">
+        <v>16</v>
+      </c>
+      <c r="L15" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="1">
+        <v>30</v>
+      </c>
+      <c r="F16" s="1">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1">
+        <v>18</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K16" s="1">
+        <v>8</v>
+      </c>
+      <c r="L16" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1166,7 +1456,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,8 +1471,8 @@
     <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="18" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" style="18" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1216,119 +1506,127 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="17" t="s">
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="10">
+      <c r="A2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5">
+        <v>15</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11">
+        <v>30</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4">
         <v>5</v>
-      </c>
-      <c r="F2" s="9">
-        <v>32</v>
-      </c>
-      <c r="G2" s="9">
-        <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="L2" s="9">
-        <v>3.2000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="10">
-        <v>10</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9">
+        <v>31</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="15">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
         <v>30</v>
       </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9">
+      <c r="F4" s="9"/>
+      <c r="G4" s="9">
+        <v>35</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="9"/>
+      <c r="L4" s="15">
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="10">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4">
         <v>5</v>
       </c>
-      <c r="F4" s="9">
-        <v>19</v>
-      </c>
-      <c r="G4" s="9">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K4" s="9">
-        <v>2</v>
-      </c>
-      <c r="L4" s="9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="10">
-        <v>30</v>
-      </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="9">
+        <v>27</v>
+      </c>
       <c r="G5" s="9">
-        <v>34</v>
-      </c>
-      <c r="J5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9">
-        <v>0.125</v>
+        <v>41</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="9">
+        <v>1</v>
+      </c>
+      <c r="L5" s="14">
+        <v>6.4000000000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1338,9 +1636,9 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
@@ -1356,7 +1654,8 @@
     <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.42578125" style="18" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" style="17" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1390,91 +1689,99 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="17" t="s">
+      <c r="K1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E2" s="10">
-        <v>10</v>
-      </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10">
-        <v>24</v>
+        <v>5</v>
+      </c>
+      <c r="F2" s="9">
+        <v>32</v>
+      </c>
+      <c r="G2" s="9">
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20">
-        <v>0.25</v>
+        <v>66</v>
+      </c>
+      <c r="K2" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="L2" s="9">
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="E3" s="10">
         <v>10</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10">
-        <v>24</v>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9">
+        <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>98</v>
-      </c>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20" t="s">
-        <v>92</v>
+        <v>26</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9">
+        <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="E4" s="10">
-        <v>30</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10">
-        <v>24</v>
+        <v>5</v>
+      </c>
+      <c r="F4" s="9">
+        <v>19</v>
+      </c>
+      <c r="G4" s="9">
+        <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="K4" s="9">
+        <v>2</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -1485,116 +1792,53 @@
       <c r="E5" s="10">
         <v>30</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10">
-        <v>24</v>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9">
+        <v>34</v>
       </c>
       <c r="J5" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20" t="s">
+      <c r="K5" s="9"/>
+      <c r="L5" s="9">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="30">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="10">
-        <v>30</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="J7" t="s">
-        <v>99</v>
-      </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="10">
-        <v>30</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10">
-        <v>21</v>
-      </c>
-      <c r="J8" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="10">
-        <v>30</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20" t="s">
-        <v>94</v>
+      <c r="L7" s="17" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1602,12 +1846,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,6 +1891,680 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="18">
+        <v>30</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="K2" s="10">
+        <v>8</v>
+      </c>
+      <c r="L2" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="18">
+        <v>10</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="11">
+        <v>24</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="10">
+        <v>8</v>
+      </c>
+      <c r="L3" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10">
+        <v>10</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="10">
+        <v>1</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10">
+        <v>10</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="10">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10">
+        <v>10</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="10">
+        <v>4</v>
+      </c>
+      <c r="L6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10">
+        <v>30</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10">
+        <v>5</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10">
+        <v>30</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="4">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4">
+        <v>24</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4">
+        <v>30</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4">
+        <v>24</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.42578125" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="10">
+        <v>10</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="10">
+        <v>10</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="10">
+        <v>30</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="10">
+        <v>30</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="10">
+        <v>30</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="18"/>
+      <c r="J7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="10">
+        <v>30</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="10">
+        <v>30</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="4">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4">
+        <v>18</v>
+      </c>
+      <c r="G10" s="4">
+        <v>22</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="4">
+        <v>8</v>
+      </c>
+      <c r="L10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="10">
+        <v>10</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="J11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" t="s">
+        <v>124</v>
+      </c>
+      <c r="J12" t="s">
+        <v>125</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1654,49 +2572,47 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5">
+        <v>30</v>
+      </c>
+      <c r="F2" s="5">
+        <v>16</v>
+      </c>
+      <c r="G2" s="5">
+        <v>20</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="6">
+        <v>16</v>
+      </c>
+      <c r="L2" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="4">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4">
-        <v>15</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="4">
-        <v>16</v>
-      </c>
-      <c r="L2" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>15</v>
@@ -1705,68 +2621,70 @@
         <v>10</v>
       </c>
       <c r="F3" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="4">
+        <v>8</v>
+      </c>
+      <c r="L3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4">
         <v>17</v>
-      </c>
-      <c r="K3" s="4">
-        <v>16</v>
-      </c>
-      <c r="L3" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="4">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4">
-        <v>19</v>
-      </c>
-      <c r="G4" s="4">
-        <v>23</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K4" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>25</v>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="E5" s="4">
         <v>10</v>
       </c>
@@ -1779,7 +2697,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K5" s="4">
         <v>4</v>
@@ -1788,36 +2706,360 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4">
         <v>10</v>
       </c>
       <c r="F6" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="4">
+        <v>4</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4">
+        <v>22</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K7" s="4">
         <v>2</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L7" s="4">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4">
+        <v>30</v>
+      </c>
+      <c r="F8" s="4">
+        <v>17</v>
+      </c>
+      <c r="G8" s="4">
+        <v>21</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="4">
+        <v>16</v>
+      </c>
+      <c r="L8" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="4">
+        <v>30</v>
+      </c>
+      <c r="F9" s="4">
+        <v>22</v>
+      </c>
+      <c r="G9" s="4">
+        <v>26</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="4">
+        <v>4</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="4">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4">
+        <v>19</v>
+      </c>
+      <c r="G10" s="4">
+        <v>23</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="4">
+        <v>4</v>
+      </c>
+      <c r="L10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4">
+        <v>30</v>
+      </c>
+      <c r="F11" s="4">
+        <v>18</v>
+      </c>
+      <c r="G11" s="4">
+        <v>25</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="4">
+        <v>16</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1">
+        <v>21</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1">
+        <v>25</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K13" s="1">
+        <v>4</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1">
+        <v>20</v>
+      </c>
+      <c r="F14" s="1">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1">
+        <v>18</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K14" s="1">
+        <v>16</v>
+      </c>
+      <c r="L14" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
+        <v>30</v>
+      </c>
+      <c r="F15" s="1">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1">
+        <v>16</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K15" s="1">
+        <v>16</v>
+      </c>
+      <c r="L15" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1">
+        <v>30</v>
+      </c>
+      <c r="F16" s="1">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1">
+        <v>18</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K16" s="1">
+        <v>8</v>
+      </c>
+      <c r="L16" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1827,10 +3069,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:H9"/>
+      <selection activeCell="C2" sqref="C2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,6 +3195,36 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K4" s="1">
+        <v>16</v>
+      </c>
+      <c r="L4" s="1">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1960,16 +3232,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B10" sqref="B10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
@@ -2106,7 +3378,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -2114,10 +3386,10 @@
         <v>17</v>
       </c>
       <c r="K4" s="4">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L4" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2154,7 +3426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>45</v>
       </c>
@@ -2184,6 +3456,131 @@
       </c>
       <c r="L6" s="4">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" s="1">
+        <v>16</v>
+      </c>
+      <c r="L7" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1">
+        <v>23</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K8" s="1">
+        <v>8</v>
+      </c>
+      <c r="L8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1">
+        <v>18</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" s="1">
+        <v>16</v>
+      </c>
+      <c r="L9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="1">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1">
+        <v>21</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K10" s="1">
+        <v>16</v>
+      </c>
+      <c r="L10" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2193,10 +3590,130 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5">
+        <v>25</v>
+      </c>
+      <c r="F2" s="5">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="6">
+        <v>4</v>
+      </c>
+      <c r="L2" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,17 +3897,86 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="24">
+        <v>10</v>
+      </c>
+      <c r="F7" s="24">
+        <v>16</v>
+      </c>
+      <c r="G7" s="24">
+        <v>17</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="24">
+        <v>16</v>
+      </c>
+      <c r="L7" s="24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="24">
+        <v>10</v>
+      </c>
+      <c r="F8" s="24">
+        <v>14</v>
+      </c>
+      <c r="G8" s="24">
+        <v>15</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8" s="24">
+        <v>16</v>
+      </c>
+      <c r="L8" s="24">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2469,10 +4055,10 @@
         <v>63</v>
       </c>
       <c r="K2" s="6">
+        <v>8</v>
+      </c>
+      <c r="L2" s="6">
         <v>4</v>
-      </c>
-      <c r="L2" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2505,6 +4091,114 @@
       </c>
       <c r="L3" s="4">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4">
+        <v>18</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="4">
+        <v>16</v>
+      </c>
+      <c r="L6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2512,12 +4206,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2592,7 +4286,7 @@
         <v>20</v>
       </c>
       <c r="G2" s="5">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -2621,10 +4315,10 @@
         <v>15</v>
       </c>
       <c r="F3" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G3" s="4">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -2635,7 +4329,7 @@
         <v>32</v>
       </c>
       <c r="L3" s="4">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2701,229 +4395,6 @@
       <c r="L5" s="4">
         <v>1</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="10">
-        <v>10</v>
-      </c>
-      <c r="F2" s="12">
-        <v>18</v>
-      </c>
-      <c r="G2" s="12">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" s="12">
-        <v>4</v>
-      </c>
-      <c r="L2" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="J3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="12">
-        <v>8</v>
-      </c>
-      <c r="L3" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="10">
-        <v>5</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="10">
-        <v>5</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>87</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="10">
-        <v>30</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12">
-        <v>26</v>
-      </c>
-      <c r="J6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="10">
-        <v>10</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11">
-        <v>20</v>
-      </c>
-      <c r="J7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2932,26 +4403,26 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2993,119 +4464,174 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5">
-        <v>15</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="10">
+        <v>10</v>
+      </c>
+      <c r="F2" s="12">
+        <v>18</v>
+      </c>
+      <c r="G2" s="12">
+        <v>22</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="12">
+        <v>4</v>
+      </c>
+      <c r="L2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="J3" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="12">
+        <v>8</v>
+      </c>
+      <c r="L3" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="10">
+        <v>5</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12">
+        <v>21</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="10">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12">
+        <v>17</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="10">
         <v>30</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4">
-        <v>5</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9">
-        <v>31</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="16">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4">
+      <c r="F6" s="12"/>
+      <c r="G6" s="12">
+        <v>26</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="10">
+        <v>10</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11">
+        <v>20</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="1">
         <v>30</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9">
-        <v>35</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="16">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4">
-        <v>5</v>
-      </c>
-      <c r="F5" s="9">
-        <v>27</v>
-      </c>
-      <c r="G5" s="9">
-        <v>41</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="K5" s="9">
-        <v>1</v>
-      </c>
-      <c r="L5" s="15">
-        <v>6.4000000000000001E-2</v>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>